<commit_message>
fixed url incompleta di url documento in filtered metaglossario, cambiato set terminologia da ITCH00000 nel foglio excel di input in numeri assegnati
</commit_message>
<xml_diff>
--- a/static/saved_dataframes/tabelle_entita_e_relazionali/Things.xlsx
+++ b/static/saved_dataframes/tabelle_entita_e_relazionali/Things.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C399"/>
+  <dimension ref="A1:C403"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -820,7 +820,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>SOREU dei laghi</t>
+          <t>Centrale nazionale d'allarme</t>
         </is>
       </c>
     </row>
@@ -833,7 +833,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Vigili del fuoco</t>
+          <t>Stato maggiore federale Protezione della popolazione</t>
         </is>
       </c>
     </row>
@@ -846,7 +846,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Nucleo Unitario di Valutazione e Risposta Emergenze transfrontaliere</t>
+          <t>Protezione civile</t>
         </is>
       </c>
     </row>
@@ -855,11 +855,11 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>1000037</v>
+        <v>1000038</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Sala Operativa Regionale dell'Emergenza Urgenza</t>
+          <t>Comando della protezione civile</t>
         </is>
       </c>
     </row>
@@ -868,11 +868,11 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>1000038</v>
+        <v>1000039</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>sezione del militare e della protezione della popolazione</t>
+          <t>Impianto di protezione per la protezione della popolazione</t>
         </is>
       </c>
     </row>
@@ -881,11 +881,11 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>1000039</v>
+        <v>1000040</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Centrale nazionale d'allarme</t>
+          <t>Evento NBC</t>
         </is>
       </c>
     </row>
@@ -894,11 +894,11 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>1000040</v>
+        <v>1000041</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Stato maggiore federale Protezione della popolazione</t>
+          <t>Suscettibilità da Frana</t>
         </is>
       </c>
     </row>
@@ -907,11 +907,11 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>1000041</v>
+        <v>1000042</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Protezione civile</t>
+          <t>Pompieri</t>
         </is>
       </c>
     </row>
@@ -920,11 +920,11 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>1000042</v>
+        <v>1000043</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Legge federale sulla protezione della popolazione e sulla protezione civile</t>
+          <t>Vigili del fuoco</t>
         </is>
       </c>
     </row>
@@ -933,11 +933,11 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>1000043</v>
+        <v>1000044</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Comando della protezione civile</t>
+          <t>Struttura operativa</t>
         </is>
       </c>
     </row>
@@ -946,11 +946,11 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>1000044</v>
+        <v>1000045</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Impianto di protezione per la protezione della popolazione</t>
+          <t>Organizzazione partner</t>
         </is>
       </c>
     </row>
@@ -959,11 +959,11 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>1000045</v>
+        <v>1000046</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Evento NBC</t>
+          <t>Organo di condotta</t>
         </is>
       </c>
     </row>
@@ -972,11 +972,11 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>1000046</v>
+        <v>1000047</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Suscettibilità da Frana</t>
+          <t>Stato di necessità</t>
         </is>
       </c>
     </row>
@@ -985,11 +985,11 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>1000047</v>
+        <v>1000048</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Pompieri</t>
+          <t>Emergenza / Stato di emergenza / Evento emergenziale / Evento</t>
         </is>
       </c>
     </row>
@@ -1002,7 +1002,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Struttura operativa</t>
+          <t>Impianto di protezione</t>
         </is>
       </c>
     </row>
@@ -1015,7 +1015,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Organizzazione partner</t>
+          <t>Costruzione di protezione</t>
         </is>
       </c>
     </row>
@@ -1028,7 +1028,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Organo di condotta</t>
+          <t>Rifugio</t>
         </is>
       </c>
     </row>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Emergenza / Stato di emergenza / Evento emergenziale / Evento</t>
+          <t>Addetto all'assistenza</t>
         </is>
       </c>
     </row>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Stato di necessità</t>
+          <t>Assistente di stato maggiore</t>
         </is>
       </c>
     </row>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Impianto di protezione</t>
+          <t>Organizzazione degli Stati maggiori di condotta</t>
         </is>
       </c>
     </row>
@@ -1080,7 +1080,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Costruzione di protezione</t>
+          <t>Pioniere</t>
         </is>
       </c>
     </row>
@@ -1093,7 +1093,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Rifugio</t>
+          <t>Stato maggiore cantonale di condotta</t>
         </is>
       </c>
     </row>
@@ -1106,7 +1106,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Addetto all'assistenza</t>
+          <t>Sistema d’allarme acqua</t>
         </is>
       </c>
     </row>
@@ -1119,7 +1119,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Assistente di stato maggiore</t>
+          <t>Allarme acqua</t>
         </is>
       </c>
     </row>
@@ -1132,7 +1132,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Organizzazione degli Stati maggiori di condotta</t>
+          <t>Stato maggiore regionale di condotta</t>
         </is>
       </c>
     </row>
@@ -1145,7 +1145,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Pioniere</t>
+          <t>Stato maggiore enti di primo intervento</t>
         </is>
       </c>
     </row>
@@ -1154,11 +1154,11 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>1000061</v>
+        <v>1000062</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Stato maggiore cantonale di condotta</t>
+          <t>Protezione della popolazione</t>
         </is>
       </c>
     </row>
@@ -1167,11 +1167,11 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>1000062</v>
+        <v>1000063</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Sistema d’allarme acqua</t>
+          <t>Dipartimento della protezione civile</t>
         </is>
       </c>
     </row>
@@ -1180,11 +1180,11 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>1000063</v>
+        <v>1000064</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Allarme acqua</t>
+          <t>Legge federale sulla protezione della popolazione e sulla protezione civile</t>
         </is>
       </c>
     </row>
@@ -1193,11 +1193,11 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>1000064</v>
+        <v>1000066</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Stato maggiore regionale di condotta</t>
+          <t>Volontario di protezione civile</t>
         </is>
       </c>
     </row>
@@ -1206,11 +1206,11 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>1000065</v>
+        <v>1000068</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Stato maggiore enti di primo intervento</t>
+          <t>Consiglio di stato</t>
         </is>
       </c>
     </row>
@@ -1219,11 +1219,11 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>1000066</v>
+        <v>1000069</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Protezione della popolazione</t>
+          <t>Milite</t>
         </is>
       </c>
     </row>
@@ -1232,11 +1232,11 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>1000068</v>
+        <v>1000070</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Dipartimento della protezione civile</t>
+          <t>Legge sulla protezione della popolazione del 26 febbraio 2007</t>
         </is>
       </c>
     </row>
@@ -1245,11 +1245,11 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>1000069</v>
+        <v>1000071</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Legge sulla protezione della popolazione del 26 febbraio 2007</t>
+          <t>Nucleo Unitario di Valutazione e Risposta Emergenze transfrontaliere</t>
         </is>
       </c>
     </row>
@@ -1258,11 +1258,11 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>1000071</v>
+        <v>1000073</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Volontario di protezione civile</t>
+          <t>Sala Operativa Regionale dell'Emergenza Urgenza</t>
         </is>
       </c>
     </row>
@@ -1271,11 +1271,11 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>1000073</v>
+        <v>1000074</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Consiglio di stato</t>
+          <t>SOREU dei laghi</t>
         </is>
       </c>
     </row>
@@ -1284,11 +1284,11 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>1000074</v>
+        <v>1000075</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Milite</t>
+          <t>sezione del militare e della protezione della popolazione</t>
         </is>
       </c>
     </row>
@@ -1739,7 +1739,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>La SOREU dei Laghi è il riferimento per i territori di Como, Varese, Lecco e l'area del Legnanese.</t>
+          <t>La CENAL, una divisione dell'Ufficio federale della protezione della popolazione (UFPP), è l'organo federale competente per gli eventi straordinari. Il compito principale della CENAL è quello di tracciare il quadro della situazione prioritaria per la protezione della popolazione. A tal fine, sia nella quotidianità che in caso d'evento scambia informazioni con le autorità competenti dei Cantoni, diversi uffici federali, i gestori delle reti di telecomunicazione, dell'energia e dei trasporti, organizzazioni internazionali e con i centri d'analisi della situazione dei Paesi limitrofi. In caso d'evento, funge da primo punto di contatto per i Cantoni in relazione a tutte le questioni inerenti alla protezione della popolazione. In caso di eventi maggiori, la CENAL informa lo stato maggiore federale Protezione della popolazione e l'assiste nel suo lavoro.</t>
         </is>
       </c>
     </row>
@@ -1751,76 +1751,6 @@
         <v>3000035</v>
       </c>
       <c r="C107" t="inlineStr">
-        <is>
-          <t>Struttura operativa della protezione civile.</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" s="1" t="n">
-        <v>106</v>
-      </c>
-      <c r="B108" t="n">
-        <v>3000036</v>
-      </c>
-      <c r="C108" t="inlineStr">
-        <is>
-          <t>team transfrontaliero di coordinamento costituito congiuntamente da personale qualificato, formato e attrezzato, della protezione civile lombarda e ticinese. Esso ha il compito, durante le emergenze nei territori di confine, di operare insieme sia per la valutazione dell’evento in corso e per i reciproci possibili riflessi sui rispettivi territori, sia quali “ufficiali di collegamento” per collegare le rispettive sale operative di ambo i lati del confine, consentendo una efficiente ed efficace relazione operativa. Il NUVRE viene introdotto dal progetto Gestisco 2018-2021.</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" s="1" t="n">
-        <v>107</v>
-      </c>
-      <c r="B109" t="n">
-        <v>3000037</v>
-      </c>
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>Le SOREU hanno valenza interprovinciale: gestiscono le chiamate di soccorso sanitario con l'invio dei mezzi più appropriati fino al completamento del soccorso e/o all'eventuale affidamento del paziente alle strutture ospedaliere più idonee. Le SOREU operano tramite le dotazioni tecnologiche assegnate da AREU che permettono loro una costante interconnessione con i Call Center NUE 112 di riferimento, con i mezzi di soccorso delle AAT della propria area di competenza e con i Call Center sanitari specialistici, in modo da ottimizzare i tempi di risposta e intervento.</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" s="1" t="n">
-        <v>108</v>
-      </c>
-      <c r="B110" t="n">
-        <v>3000038</v>
-      </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>La Sezione è articolata in cinque servizi con distinte aree di competenza: il Servizio amministrativo, il Servizio degli affari militari e del comando di circondario, il Servizio della protezione civile, il Servizio costruzioni di protezione civile e il Servizio della protezione della popolazione. 
-Il servizio amministrativo centralizzato della sezione si occupa di fornire le prime informazioni all’utenza e di smistarle ai vari servizi di competenza. Altri compiti specifici sono la contabilità, la corrispondenza e il supporto logistico per tutta la sezione. 
-Il Servizio degli affari militari e comando di circondario si occupa delle pratiche amministrative legate ai servizi d’istruzione dei militi domiciliati in Ticino come pure degli obblighi fuori servizio (tiro obbligatorio, obbligo di notifica), tiene il controllo dei dati di servizio e di quelli personali dei militi con la collaborazione degli uffici di controllo abitanti dei comuni. 
-Il Servizio della protezione civile, unitamente al Centro istruzione della protezione civile di Rivera, assicura l'applicazione delle norme federali e cantonali di protezione civile nelle regioni e nei comuni, cura le diverse pianificazioni (allarmi, approvvigionamenti,...) e l'istruzione dei militi astretti.
-Il Servizio costruzioni si occupa della pianificazione e gestione dei posti protetti, come pure della realizzazione delle costruzioni protette (rifugi, impianti regionali).
-Il servizio della protezione della popolazione si occupa prevalentemente dei preparativi per i casi di emergenza e di catastrofe.</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" s="1" t="n">
-        <v>109</v>
-      </c>
-      <c r="B111" t="n">
-        <v>3000039</v>
-      </c>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>La CENAL, una divisione dell'Ufficio federale della protezione della popolazione (UFPP), è l'organo federale competente per gli eventi straordinari. Il compito principale della CENAL è quello di tracciare il quadro della situazione prioritaria per la protezione della popolazione. A tal fine, sia nella quotidianità che in caso d'evento scambia informazioni con le autorità competenti dei Cantoni, diversi uffici federali, i gestori delle reti di telecomunicazione, dell'energia e dei trasporti, organizzazioni internazionali e con i centri d'analisi della situazione dei Paesi limitrofi. In caso d'evento, funge da primo punto di contatto per i Cantoni in relazione a tutte le questioni inerenti alla protezione della popolazione. In caso di eventi maggiori, la CENAL informa lo stato maggiore federale Protezione della popolazione e l'assiste nel suo lavoro.</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" s="1" t="n">
-        <v>110</v>
-      </c>
-      <c r="B112" t="n">
-        <v>3000040</v>
-      </c>
-      <c r="C112" t="inlineStr">
         <is>
           <t>Nel caso in cui si delinea o si è verificato un evento di portata nazionale rilevante per la protezione della popolazione, lo SMFP assume i compiti seguenti (art. 4, cpv. 2 OSMFP):
 - assicura lo scambio di informazioni e il coordinamento con altri stati maggiori e organi della Confederazione e dei Cantoni, con i gestori di infrastrutture critiche e con i competenti organi all'estero;
@@ -1832,40 +1762,40 @@
         </is>
       </c>
     </row>
-    <row r="113">
-      <c r="A113" s="1" t="n">
-        <v>111</v>
-      </c>
-      <c r="B113" t="n">
-        <v>3000041</v>
-      </c>
-      <c r="C113" t="inlineStr">
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="B108" t="n">
+        <v>3000036</v>
+      </c>
+      <c r="C108" t="inlineStr">
         <is>
           <t>La protezione civile protegge la popolazione, assiste le persone in cerca di protezione, protegge i beni culturali, sostiene gli organi di condotta e le altre organizzazioni partner nonché svolge lavori di ripristino e di pubblica utilità. Essa è un’organizzazione civile che opera singolarmente o in maniera coordinata, come organizzazione partner, all'interno della struttura svizzera di di protezione della popolazione.</t>
         </is>
       </c>
     </row>
-    <row r="114">
-      <c r="A114" s="1" t="n">
-        <v>112</v>
-      </c>
-      <c r="B114" t="n">
-        <v>3000042</v>
-      </c>
-      <c r="C114" t="inlineStr">
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="B109" t="n">
+        <v>3000037</v>
+      </c>
+      <c r="C109" t="inlineStr">
         <is>
           <t>Il Servizio nazionale della protezione civile, di seguito Servizio nazionale, definito di pubblica utilita', e' il sistema che esercita la funzione di protezione civile costituita dall'insieme delle competenze e delle attivita' volte a tutelare la vita, l'integrita' fisica, i beni, gli insediamenti, gli animali e l'ambiente dai danni o dal pericolo di danni derivanti da eventi calamitosi di origine naturale o derivanti dall'attivita' dell'uomo.</t>
         </is>
       </c>
     </row>
-    <row r="115">
-      <c r="A115" s="1" t="n">
-        <v>113</v>
-      </c>
-      <c r="B115" t="n">
-        <v>3000043</v>
-      </c>
-      <c r="C115" t="inlineStr">
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="B110" t="n">
+        <v>3000038</v>
+      </c>
+      <c r="C110" t="inlineStr">
         <is>
           <t>Il comando della protezione civile è l’organo che dirige la protezione civile, ed è generalmente costituito dal comandante della protezione civile e dai suoi sostituti. I suoi compiti fondamentali sono i seguenti:
 - condurre gli interventi
@@ -1876,27 +1806,27 @@
         </is>
       </c>
     </row>
-    <row r="116">
-      <c r="A116" s="1" t="n">
-        <v>114</v>
-      </c>
-      <c r="B116" t="n">
-        <v>3000044</v>
-      </c>
-      <c r="C116" t="inlineStr">
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>109</v>
+      </c>
+      <c r="B111" t="n">
+        <v>3000039</v>
+      </c>
+      <c r="C111" t="inlineStr">
         <is>
           <t>Si definiscono impianti di protezione i posti di comando, gli impianti d'apprestamento, i centri sanitari protetti e gli ospedali protetti. Essi vengono utilizzati soprattutto per garantire la condotta e l’operatività dei mezzi della protezione della popolazione.</t>
         </is>
       </c>
     </row>
-    <row r="117">
-      <c r="A117" s="1" t="n">
-        <v>115</v>
-      </c>
-      <c r="B117" t="n">
-        <v>3000045</v>
-      </c>
-      <c r="C117" t="inlineStr">
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="B112" t="n">
+        <v>3000040</v>
+      </c>
+      <c r="C112" t="inlineStr">
         <is>
           <t>Per evento NBC s'intende l'emissione illecita di sostanze nucleari (atomiche e radiologiche, N), biologiche (B) o chimiche (C). L'emissione può essere accidentale (incidente) o intenzionale (atto criminale o terroristico). Si distinguono i seguenti settori:
 - settore N: emissione di radiazioni ionizzanti e radioattività;
@@ -1905,6 +1835,71 @@
         </is>
       </c>
     </row>
+    <row r="113">
+      <c r="A113" s="1" t="n">
+        <v>111</v>
+      </c>
+      <c r="B113" t="n">
+        <v>3000041</v>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>La suscettibilità da frana è la probabilità che una frana avvenga in un territorio, sulla base delle condizioni locali. E’ una misura del grado in cui un territorio potrà essere interessato da frane, ossia una stima di “dove” le frane potranno accadere. La suscettibilità non considera la ricorrenza temporale, né la dimensione delle frane. In termini matematici, la suscettibilità da frana è comunemente espressa come la probabilità d’occorrenza spaziale di un dissesto, dato un insieme di condizioni territoriali e ambientali.</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="n">
+        <v>112</v>
+      </c>
+      <c r="B114" t="n">
+        <v>3000042</v>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>I pompieri sono responsabili di salvataggio e lotta contro i sinistri in generale, compresa la lotta antincendio e contro i sinistri ordinari. Intervengono anche in caso d’emissioni tossiche, fuoriuscite di carburanti e contaminazioni radioattive. Sono un mezzo di primo intervento.</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="B115" t="n">
+        <v>3000043</v>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>In occasione degli eventi calamitosi, il Corpo nazionale dei vigili del fuoco opera gli interventi di soccorso tecnico indifferibili e urgenti: di ricerca e salvataggio delle persone e – ai fini della salvaguardia della pubblica incolumità – anche di messa in sicurezza dei luoghi, delle strutture e degli impianti.</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="n">
+        <v>114</v>
+      </c>
+      <c r="B116" t="n">
+        <v>3000044</v>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Oltre al Corpo nazionale dei vigili del fuoco, che opera quale componente fondamentale del Servizio nazionale della protezione civile, sono strutture operative nazionali: a) le Forze armate; b) le Forze di polizia; c) gli enti e istituti di ricerca di rilievo nazionale con finalità di protezione civile, anche organizzati come centri di competenza, l'Istituto nazionale di geofisica e vulcanologia e il Consiglio nazionale delle ricerche; d) le strutture del Servizio sanitario nazionale; e) il volontariato organizzato di protezione civile iscritto nell'elenco nazionale del volontariato di protezione civile, l'Associazione della Croce rossa italiana e il Corpo nazionale del soccorso alpino e speleologico; f) il Sistema nazionale per la protezione dell'ambiente; g) le strutture preposte alla gestione dei servizi meteorologici a livello nazionale.</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n">
+        <v>115</v>
+      </c>
+      <c r="B117" t="n">
+        <v>3000045</v>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Sono organizzazioni partner quelle che collaborano alla protezione della popolazione: Polizia, pompieri, servizi della sanità pubblica, servizi tecnici, protezione civile.</t>
+        </is>
+      </c>
+    </row>
     <row r="118">
       <c r="A118" s="1" t="n">
         <v>116</v>
@@ -1914,7 +1909,8 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>La suscettibilità da frana è la probabilità che una frana avvenga in un territorio, sulla base delle condizioni locali. E’ una misura del grado in cui un territorio potrà essere interessato da frane, ossia una stima di “dove” le frane potranno accadere. La suscettibilità non considera la ricorrenza temporale, né la dimensione delle frane. In termini matematici, la suscettibilità da frana è comunemente espressa come la probabilità d’occorrenza spaziale di un dissesto, dato un insieme di condizioni territoriali e ambientali.</t>
+          <t>Gli organi di condotta vengono istituiti dalle autorità competenti per lo svolgimento dei seguenti compiti: a - informare la popolazione in merito ai pericoli che la minacciano come pure alle possibilità e alle misure di protezione esistenti; b - avvertire, dare l’allarme e impartire alla popolazione istruzioni sul comportamento; c - assicurare le attività di condotta; d - coordinare i preparativi e gli interventi delle 
+ organizzazioni partner; e - garantire, tempestivamente e in funzione della situazione, la disponibilità operativa e il rinforzo con personale e materiale della protezione della popolazione in vista di un conflitto armato.</t>
         </is>
       </c>
     </row>
@@ -1927,7 +1923,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>I pompieri sono responsabili di salvataggio e lotta contro i sinistri in generale, compresa la lotta antincendio e contro i sinistri ordinari. Intervengono anche in caso d’emissioni tossiche, fuoriuscite di carburanti e contaminazioni radioattive. Sono un mezzo di primo intervento.</t>
+          <t>Si ha stato di necessità quando, a seguito di catastrofi, conflitti armati o altre situazioni d’emergenza che comportano un pericolo imminente per lo Stato, le persone o le cose, non sia più possibile garantire con i mezzi ordinari l’attività amministrativa o i servizi d’interesse pubblico e la protezione e l’assistenza delle persone e delle cose a livello cantonale, regionale o locale.</t>
         </is>
       </c>
     </row>
@@ -1940,7 +1936,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>In occasione degli eventi calamitosi, il Corpo nazionale dei vigili del fuoco opera gli interventi di soccorso tecnico indifferibili e urgenti: di ricerca e salvataggio delle persone e – ai fini della salvaguardia della pubblica incolumità – anche di messa in sicurezza dei luoghi, delle strutture e degli impianti.</t>
+          <t>Indica l'insieme delle emergenze di tipo A, B e C così come definiti dall' Art. 7, comma 1 del DL 02/01/2018, n°1.</t>
         </is>
       </c>
     </row>
@@ -1953,7 +1949,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Oltre al Corpo nazionale dei vigili del fuoco, che opera quale componente fondamentale del Servizio nazionale della protezione civile, sono strutture operative nazionali: a) le Forze armate; b) le Forze di polizia; c) gli enti e istituti di ricerca di rilievo nazionale con finalità di protezione civile, anche organizzati come centri di competenza, l'Istituto nazionale di geofisica e vulcanologia e il Consiglio nazionale delle ricerche; d) le strutture del Servizio sanitario nazionale; e) il volontariato organizzato di protezione civile iscritto nell'elenco nazionale del volontariato di protezione civile, l'Associazione della Croce rossa italiana e il Corpo nazionale del soccorso alpino e speleologico; f) il Sistema nazionale per la protezione dell'ambiente; g) le strutture preposte alla gestione dei servizi meteorologici a livello nazionale.</t>
+          <t>Sono impianti di protezione: a - i posti di comando; b. gli impianti d’apprestamento; c - i centri sanitari protetti; d - gli ospedali protetti.</t>
         </is>
       </c>
     </row>
@@ -1966,7 +1962,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Sono organizzazioni partner quelle che collaborano alla protezione della popolazione: Polizia, pompieri, servizi della sanità pubblica, servizi tecnici, protezione civile.</t>
+          <t>Le Costruzioni di protezione si distinguono in rifugi e impianti di protezione. Sono edifici che vengono costruiti o utilizzati ai fini di protezione della popolazione.</t>
         </is>
       </c>
     </row>
@@ -1979,8 +1975,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Gli organi di condotta vengono istituiti dalle autorità competenti per lo svolgimento dei seguenti compiti: a - informare la popolazione in merito ai pericoli che la minacciano come pure alle possibilità e alle misure di protezione esistenti; b - avvertire, dare l’allarme e impartire alla popolazione istruzioni sul comportamento; c - assicurare le attività di condotta; d - coordinare i preparativi e gli interventi delle 
- organizzazioni partner; e - garantire, tempestivamente e in funzione della situazione, la disponibilità operativa e il rinforzo con personale e materiale della protezione della popolazione in vista di un conflitto armato.</t>
+          <t>posto protetto di cui ogni abitante deve disporre e che sia raggiungibile in tempo utile dalla propria abitazione.</t>
         </is>
       </c>
     </row>
@@ -1993,7 +1988,7 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Indica l'insieme delle emergenze di tipo A, B e C così come definiti dall' Art. 7, comma 1 del DL 02/01/2018, n°1.</t>
+          <t>milite impiegato, in funzione dell'evento o della situazione d'emergenza, per assistere persone in cerca di protezione (senzatetto, evacuati, ecc.) o aiutare i servizi della sanità pubblica (per es. in case per anziani). L'addetto all'assistenza deve disporre di buone competenze sociali e capacità organizzative.</t>
         </is>
       </c>
     </row>
@@ -2006,7 +2001,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Si ha stato di necessità quando, a seguito di catastrofi, conflitti armati o altre situazioni d’emergenza che comportano un pericolo imminente per lo Stato, le persone o le cose, non sia più possibile garantire con i mezzi ordinari l’attività amministrativa o i servizi d’interesse pubblico e la protezione e l’assistenza delle persone e delle cose a livello cantonale, regionale o locale.</t>
+          <t>milite impiegato per prestare aiuto alla condotta in seno all'organo di condotta o a favore dei partner ed istruito in materia di analisi della situazione e telematica. L'assistente di stato maggiore deve essere polivalente.</t>
         </is>
       </c>
     </row>
@@ -2019,7 +2014,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Sono impianti di protezione: a - i posti di comando; b. gli impianti d’apprestamento; c - i centri sanitari protetti; d - gli ospedali protetti.</t>
+          <t>L’Organizzazione degli Stati maggiori di condotta (OSMC) è composta dai rappresentanti della Polizia cantonale, della Federazione cantonale ticinese corpi pompieri, della Federazione cantonale ticinese servizi autoambulanze, del Servizio della protezione civile cantonale, dei servizi tecnici e del Dipartimento delle istituzioni; ogni organizzazione designa il proprio rappresentante. A seconda delle necessità possono essere designati ulteriori responsabili per i servizi tecnici. L’OSMC è diretta dal rappresentante del Dipartimento.</t>
         </is>
       </c>
     </row>
@@ -2031,71 +2026,6 @@
         <v>3000055</v>
       </c>
       <c r="C127" t="inlineStr">
-        <is>
-          <t>Le Costruzioni di protezione si distinguono in rifugi e impianti di protezione. Sono edifici che vengono costruiti o utilizzati ai fini di protezione della popolazione.</t>
-        </is>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" s="1" t="n">
-        <v>126</v>
-      </c>
-      <c r="B128" t="n">
-        <v>3000056</v>
-      </c>
-      <c r="C128" t="inlineStr">
-        <is>
-          <t>posto protetto di cui ogni abitante deve disporre e che sia raggiungibile in tempo utile dalla propria abitazione.</t>
-        </is>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" s="1" t="n">
-        <v>127</v>
-      </c>
-      <c r="B129" t="n">
-        <v>3000057</v>
-      </c>
-      <c r="C129" t="inlineStr">
-        <is>
-          <t>milite impiegato, in funzione dell'evento o della situazione d'emergenza, per assistere persone in cerca di protezione (senzatetto, evacuati, ecc.) o aiutare i servizi della sanità pubblica (per es. in case per anziani). L'addetto all'assistenza deve disporre di buone competenze sociali e capacità organizzative.</t>
-        </is>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" s="1" t="n">
-        <v>128</v>
-      </c>
-      <c r="B130" t="n">
-        <v>3000058</v>
-      </c>
-      <c r="C130" t="inlineStr">
-        <is>
-          <t>milite impiegato per prestare aiuto alla condotta in seno all'organo di condotta o a favore dei partner ed istruito in materia di analisi della situazione e telematica. L'assistente di stato maggiore deve essere polivalente.</t>
-        </is>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" s="1" t="n">
-        <v>129</v>
-      </c>
-      <c r="B131" t="n">
-        <v>3000059</v>
-      </c>
-      <c r="C131" t="inlineStr">
-        <is>
-          <t>L’Organizzazione degli Stati maggiori di condotta (OSMC) è composta dai rappresentanti della Polizia cantonale, della Federazione cantonale ticinese corpi pompieri, della Federazione cantonale ticinese servizi autoambulanze, del Servizio della protezione civile cantonale, dei servizi tecnici e del Dipartimento delle istituzioni; ogni organizzazione designa il proprio rappresentante. A seconda delle necessità possono essere designati ulteriori responsabili per i servizi tecnici. L’OSMC è diretta dal rappresentante del Dipartimento.</t>
-        </is>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" s="1" t="n">
-        <v>130</v>
-      </c>
-      <c r="B132" t="n">
-        <v>3000060</v>
-      </c>
-      <c r="C132" t="inlineStr">
         <is>
           <t>milite impiegato soprattutto per assistere le organizzazioni
 partner nell'esecuzione dei lavori necessari per limitare o ripristinare i
@@ -2104,6 +2034,71 @@
         </is>
       </c>
     </row>
+    <row r="128">
+      <c r="A128" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="B128" t="n">
+        <v>3000056</v>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>Lo SMCC è l’organo cantonale di condotta del Consiglio di Stato, che ne definisce la composizione, l’organizzazione e il funzionamento. Esso elabora le basi decisionali per il Consiglio di Stato, lo coadiuva nelle funzioni di direzione e coordinamento ed esegue le sue decisioni. Esso è competente quando le circostanze lo esigono, per predisporre e coordinare, in collaborazione con le autorità locali, le necessarie misure d’urgenza e di assistenza e condurne l’attuazione. La sua attivazione è decisa dal Comandante della Polizia cantonale; in caso di impedimento di questo e in successione, dal suo sostituto o dall’ufficiale di picchetto della Polizia cantonale.</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="n">
+        <v>127</v>
+      </c>
+      <c r="B129" t="n">
+        <v>3000057</v>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>Sistema di allertamento per eventi di tipo idrometeorologico.</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="B130" t="n">
+        <v>3000058</v>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>Il segnale d'allarme acqua viene emesso esclusivamente nelle regioni minacciate a valle di impianti d'accumulazione. Le sirene emettono dodici suoni continui e gravi in sequenze di 20 secondi e a intervalli di 10 secondi. L’allarme acqua esorta la popolazione ad abbandonare immediatamente la regione minacciata.</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="B131" t="n">
+        <v>3000059</v>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>Lo SMRC è un organo di condotta che permette la coordinazione di più SMEPI attivi nella medesima regione. La costituzione di uno SMRC può essere ordinata o autorizzata dal Comandante dello SMCC. Esso è di norma condotto da un ufficiale della Polizia cantonale.</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="B132" t="n">
+        <v>3000060</v>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>Lo SMEPI coordina l’intervento dei primi enti mobilitati, di regola polizia, pompieri e servizi d’autoambulanza. Esso è condotto, di principio, dalla Polizia cantonale.</t>
+        </is>
+      </c>
+    </row>
     <row r="133">
       <c r="A133" s="1" t="n">
         <v>131</v>
@@ -2113,7 +2108,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>Lo SMCC è l’organo cantonale di condotta del Consiglio di Stato, che ne definisce la composizione, l’organizzazione e il funzionamento. Esso elabora le basi decisionali per il Consiglio di Stato, lo coadiuva nelle funzioni di direzione e coordinamento ed esegue le sue decisioni. Esso è competente quando le circostanze lo esigono, per predisporre e coordinare, in collaborazione con le autorità locali, le necessarie misure d’urgenza e di assistenza e condurne l’attuazione. La sua attivazione è decisa dal Comandante della Polizia cantonale; in caso di impedimento di questo e in successione, dal suo sostituto o dall’ufficiale di picchetto della Polizia cantonale.</t>
+          <t>La legge federale sulla protezione della popolazione e sulla protezione civile (LPPC) del 4 ottobre 2002 può essere considerata come la più importante legge dello stato svizzero in materia di protezione della protezione della popolazione, che costituisce quadro normativo di riferimento per altre leggi federali e cantonali in materia di protezione della popolazione. Essa disciplina principalmente due ambiti: - la collaborazione tra Confederazione e Cantoni nella protezione della popolazione. - il ruolo e i doveri degli organi e dei corpi della protezione della popolazione.</t>
         </is>
       </c>
     </row>
@@ -2126,7 +2121,9 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Sistema di allertamento per eventi di tipo idrometeorologico.</t>
+          <t>Il servizio della protezione della popolazione si occupa prevalentemente dei preparativi per i casi di emergenza e di catastrofe.
+Assicura la collaborazione con i servizi delle Amministrazioni: federale, cantonale e comunali direttamente collegate con i temi trattati dal servizio e si occupa della coordinazione fra i partner del concetto “protezione della popolazione” (polizia cantonale, Federazione cantonale ticinese dei Corpi Pompieri, Federazione cantonale ticinese dei Servizi autoambulanze, organizzazioni regionali di protezione civile, servizi tecnici cantonali, servizi dello Stato Maggiore cantonale di catastrofe, ecc…).
+Per il tramite di esercitazioni teoriche e pratiche, approfondisce con le istanze militari, la collaborazione civile-militare.</t>
         </is>
       </c>
     </row>
@@ -2139,7 +2136,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Il segnale d'allarme acqua viene emesso esclusivamente nelle regioni minacciate a valle di impianti d'accumulazione. Le sirene emettono dodici suoni continui e gravi in sequenze di 20 secondi e a intervalli di 10 secondi. L’allarme acqua esorta la popolazione ad abbandonare immediatamente la regione minacciata.</t>
+          <t>Il Dipartimento della protezione civile è una struttura della Presidenza del Consiglio dei Ministri. Il Dipartimento, operando in stretto raccordo con le Regioni e le Province autonome, si occupa di tutte le attività volte alla previsione e alla prevenzione dei rischi, al soccorso e all’assistenza delle popolazioni colpite da calamità, al contrasto e al superamento dell’emergenza.</t>
         </is>
       </c>
     </row>
@@ -2150,22 +2147,18 @@
       <c r="B136" t="n">
         <v>3000064</v>
       </c>
-      <c r="C136" t="inlineStr">
-        <is>
-          <t>Lo SMRC è un organo di condotta che permette la coordinazione di più SMEPI attivi nella medesima regione. La costituzione di uno SMRC può essere ordinata o autorizzata dal Comandante dello SMCC. Esso è di norma condotto da un ufficiale della Polizia cantonale.</t>
-        </is>
-      </c>
+      <c r="C136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>3000065</v>
+        <v>3000066</v>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>Lo SMEPI coordina l’intervento dei primi enti mobilitati, di regola polizia, pompieri e servizi d’autoambulanza. Esso è condotto, di principio, dalla Polizia cantonale.</t>
+          <t>Il decreto legislativo n. 1 del 2018, Codice della Protezioone Civile, include il volontariato organizzato di protezione civile iscritto nell'elenco nazionale del volontariato di protezione civile tra le strutture operative del Servizio nazionale. Il volontariato si integra con gli altri livelli territoriali di intervento previsti nell'organizzazione del sistema nazionale della protezione civile, in base al principio della sussidiarietà verticale. È inoltre attore del sistema e del proprio territorio: protegge la comunità in collaborazione con le istituzioni, in base al principio della sussidiarietà orizzontale.</t>
         </is>
       </c>
     </row>
@@ -2174,13 +2167,12 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>3000066</v>
+        <v>3000067</v>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Il servizio della protezione della popolazione si occupa prevalentemente dei preparativi per i casi di emergenza e di catastrofe.
-Assicura la collaborazione con i servizi delle Amministrazioni: federale, cantonale e comunali direttamente collegate con i temi trattati dal servizio e si occupa della coordinazione fra i partner del concetto “protezione della popolazione” (polizia cantonale, Federazione cantonale ticinese dei Corpi Pompieri, Federazione cantonale ticinese dei Servizi autoambulanze, organizzazioni regionali di protezione civile, servizi tecnici cantonali, servizi dello Stato Maggiore cantonale di catastrofe, ecc…).
-Per il tramite di esercitazioni teoriche e pratiche, approfondisce con le istanze militari, la collaborazione civile-militare.</t>
+          <t>La legge LPPC 2002 stabilisce che possono prestare volontariamente servizio di protezione civile: a. gli uomini prosciolti dall’obbligo di prestare servizio nella protezione civile; b. gli uomini soggetti all’obbligo militare prosciolti dall’obbligo di prestare servizio militare o civile; c. gli uomini prosciolti dall’obbligo di prestare servizio militare o civile; d. le cittadine svizzere, a partire dall’anno in cui compiono i 20 anni; e. gli stranieri domiciliati in Svizzera, a partire dall’anno in cui compiono i 20 anni. Bisogna porre attenzione al fatto che secondo la stessa legge, l’unica differenza tra un milite e un volontario (entrambi di protezione civile) è il fatto che i volontari sono prosciolti dall’obbligo di prestare servizio su domanda. Infatti, per il resto, militi e volontari hanno gli stessi diritti e doveri. 
+I diritti dei militi sono essenzialmente quattro: soldo e vitto, alloggio, trasporto gratuiti, cui si aggiungono alcune agevolazioni fiscali e indennità.</t>
         </is>
       </c>
     </row>
@@ -2193,7 +2185,8 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Il Dipartimento della protezione civile è una struttura della Presidenza del Consiglio dei Ministri. Il Dipartimento, operando in stretto raccordo con le Regioni e le Province autonome, si occupa di tutte le attività volte alla previsione e alla prevenzione dei rischi, al soccorso e all’assistenza delle popolazioni colpite da calamità, al contrasto e al superamento dell’emergenza.</t>
+          <t>Il Consiglio di Stato è l’autorità competente per: a) assicurare la condotta, l’intervento e il coordinamento delle organizzazioni partner; b) assicurare l’istruzione e la formazione, anche degli organi di condotta locali; c) promuovere l’aiuto intercomunale, così come la cooperazione intercantonale e
+transfrontaliera; d) esercitare le altre funzioni attribuitegli dalla presente legge.</t>
         </is>
       </c>
     </row>
@@ -2206,7 +2199,8 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>La legge federale sulla protezione della popolazione e sulla protezione civile (LPPC) del 4 ottobre 2002 può essere considerata come la più importante legge dello stato svizzero in materia di protezione della protezione della popolazione, che costituisce quadro normativo di riferimento per altre leggi federali e cantonali in materia di protezione della popolazione. Essa disciplina principalmente due ambiti: - la collaborazione tra Confederazione e Cantoni nella protezione della popolazione. - il ruolo e i doveri degli organi e dei corpi della protezione della popolazione.</t>
+          <t>I militi svizzeri sono reclutati dall’esercito e dalla protezione civile e di norma vengono assegnati al loro cantone di domicilio, oppure ad altri cantoni, se deciso dal cantone di domicilio, cui comunque spetta la scelta. I militi, oltre ad essere arruolati in maniera ordinaria, possono essere incorporati nel personale di riserva. Se un milite entra a far parte del personale di riserva non deve essere necessariamente formato e non ha diritto a prestare servizio di protezione civile.
+Una volta reclutati e addestrasti, i militi possono essere chiamati a prestare servizio dal consiglio federale o dal cantone cui sono assegnati. Il Consiglio federale e il cantone di assegnamento possono chiamare in servizio i militi di protezione civile in caso di catastrofi e situazioni d’emergenza che colpiscono uno o più Cantoni, oppure le zone limitrofe di Paesi confinanti, oppure in caso di conflitto armato. I militi possono inoltre essere mobilitati anche in assenza di emergenza per svolgere dei lavori di ripristino di pubblica utilità. In quest’ultimo caso però, esistono dei limiti al potere di convocazione esercitato dalle autorità sui militi .</t>
         </is>
       </c>
     </row>
@@ -2217,7 +2211,12 @@
       <c r="B141" t="n">
         <v>3000070</v>
       </c>
-      <c r="C141" t="inlineStr"/>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>La legge cantonale del 26 febbraio 2007 è legge di maggior riferimento del Canton Ticino in materia di protezione della popolazione.
+Essa riprende alcuni argomenti già sanciti dalla legge federale LPPC del 2002, approfondisce la struttura e i compiti di alcuni organi di protezione della popolazione cantonali, quali gli organi di condotta, e descrive il concetto di stato di necessità a livello cantonale.</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
@@ -2228,7 +2227,7 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>Il decreto legislativo n. 1 del 2018, Codice della Protezioone Civile, include il volontariato organizzato di protezione civile iscritto nell'elenco nazionale del volontariato di protezione civile tra le strutture operative del Servizio nazionale. Il volontariato si integra con gli altri livelli territoriali di intervento previsti nell'organizzazione del sistema nazionale della protezione civile, in base al principio della sussidiarietà verticale. È inoltre attore del sistema e del proprio territorio: protegge la comunità in collaborazione con le istituzioni, in base al principio della sussidiarietà orizzontale.</t>
+          <t>team transfrontaliero di coordinamento costituito congiuntamente da personale qualificato, formato e attrezzato, della protezione civile lombarda e ticinese. Esso ha il compito, durante le emergenze nei territori di confine, di operare insieme sia per la valutazione dell’evento in corso e per i reciproci possibili riflessi sui rispettivi territori, sia quali “ufficiali di collegamento” per collegare le rispettive sale operative di ambo i lati del confine, consentendo una efficiente ed efficace relazione operativa. Il NUVRE viene introdotto dal progetto Gestisco 2018-2021.</t>
         </is>
       </c>
     </row>
@@ -2241,8 +2240,7 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>La legge LPPC 2002 stabilisce che possono prestare volontariamente servizio di protezione civile: a. gli uomini prosciolti dall’obbligo di prestare servizio nella protezione civile; b. gli uomini soggetti all’obbligo militare prosciolti dall’obbligo di prestare servizio militare o civile; c. gli uomini prosciolti dall’obbligo di prestare servizio militare o civile; d. le cittadine svizzere, a partire dall’anno in cui compiono i 20 anni; e. gli stranieri domiciliati in Svizzera, a partire dall’anno in cui compiono i 20 anni. Bisogna porre attenzione al fatto che secondo la stessa legge, l’unica differenza tra un milite e un volontario (entrambi di protezione civile) è il fatto che i volontari sono prosciolti dall’obbligo di prestare servizio su domanda. Infatti, per il resto, militi e volontari hanno gli stessi diritti e doveri. 
-I diritti dei militi sono essenzialmente quattro: soldo e vitto, alloggio, trasporto gratuiti, cui si aggiungono alcune agevolazioni fiscali e indennità.</t>
+          <t>Struttura operativa della protezione civile.</t>
         </is>
       </c>
     </row>
@@ -2255,8 +2253,7 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>Il Consiglio di Stato è l’autorità competente per: a) assicurare la condotta, l’intervento e il coordinamento delle organizzazioni partner; b) assicurare l’istruzione e la formazione, anche degli organi di condotta locali; c) promuovere l’aiuto intercomunale, così come la cooperazione intercantonale e
-transfrontaliera; d) esercitare le altre funzioni attribuitegli dalla presente legge.</t>
+          <t>Le SOREU hanno valenza interprovinciale: gestiscono le chiamate di soccorso sanitario con l'invio dei mezzi più appropriati fino al completamento del soccorso e/o all'eventuale affidamento del paziente alle strutture ospedaliere più idonee. Le SOREU operano tramite le dotazioni tecnologiche assegnate da AREU che permettono loro una costante interconnessione con i Call Center NUE 112 di riferimento, con i mezzi di soccorso delle AAT della propria area di competenza e con i Call Center sanitari specialistici, in modo da ottimizzare i tempi di risposta e intervento.</t>
         </is>
       </c>
     </row>
@@ -2269,8 +2266,7 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>I militi svizzeri sono reclutati dall’esercito e dalla protezione civile e di norma vengono assegnati al loro cantone di domicilio, oppure ad altri cantoni, se deciso dal cantone di domicilio, cui comunque spetta la scelta. I militi, oltre ad essere arruolati in maniera ordinaria, possono essere incorporati nel personale di riserva. Se un milite entra a far parte del personale di riserva non deve essere necessariamente formato e non ha diritto a prestare servizio di protezione civile.
-Una volta reclutati e addestrasti, i militi possono essere chiamati a prestare servizio dal consiglio federale o dal cantone cui sono assegnati. Il Consiglio federale e il cantone di assegnamento possono chiamare in servizio i militi di protezione civile in caso di catastrofi e situazioni d’emergenza che colpiscono uno o più Cantoni, oppure le zone limitrofe di Paesi confinanti, oppure in caso di conflitto armato. I militi possono inoltre essere mobilitati anche in assenza di emergenza per svolgere dei lavori di ripristino di pubblica utilità. In quest’ultimo caso però, esistono dei limiti al potere di convocazione esercitato dalle autorità sui militi .</t>
+          <t>La SOREU dei Laghi è il riferimento per i territori di Como, Varese, Lecco e l'area del Legnanese.</t>
         </is>
       </c>
     </row>
@@ -2283,8 +2279,12 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>La legge cantonale del 26 febbraio 2007 è legge di maggior riferimento del Canton Ticino in materia di protezione della popolazione.
-Essa riprende alcuni argomenti già sanciti dalla legge federale LPPC del 2002, approfondisce la struttura e i compiti di alcuni organi di protezione della popolazione cantonali, quali gli organi di condotta, e descrive il concetto di stato di necessità a livello cantonale.</t>
+          <t>La Sezione è articolata in cinque servizi con distinte aree di competenza: il Servizio amministrativo, il Servizio degli affari militari e del comando di circondario, il Servizio della protezione civile, il Servizio costruzioni di protezione civile e il Servizio della protezione della popolazione. 
+Il servizio amministrativo centralizzato della sezione si occupa di fornire le prime informazioni all’utenza e di smistarle ai vari servizi di competenza. Altri compiti specifici sono la contabilità, la corrispondenza e il supporto logistico per tutta la sezione. 
+Il Servizio degli affari militari e comando di circondario si occupa delle pratiche amministrative legate ai servizi d’istruzione dei militi domiciliati in Ticino come pure degli obblighi fuori servizio (tiro obbligatorio, obbligo di notifica), tiene il controllo dei dati di servizio e di quelli personali dei militi con la collaborazione degli uffici di controllo abitanti dei comuni. 
+Il Servizio della protezione civile, unitamente al Centro istruzione della protezione civile di Rivera, assicura l'applicazione delle norme federali e cantonali di protezione civile nelle regioni e nei comuni, cura le diverse pianificazioni (allarmi, approvvigionamenti,...) e l'istruzione dei militi astretti.
+Il Servizio costruzioni si occupa della pianificazione e gestione dei posti protetti, come pure della realizzazione delle costruzioni protette (rifugi, impianti regionali).
+Il servizio della protezione della popolazione si occupa prevalentemente dei preparativi per i casi di emergenza e di catastrofe.</t>
         </is>
       </c>
     </row>
@@ -2367,7 +2367,7 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>4000046</v>
+        <v>4000041</v>
       </c>
       <c r="C153" t="inlineStr">
         <is>
@@ -2380,7 +2380,7 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>4000047</v>
+        <v>4000042</v>
       </c>
       <c r="C154" t="inlineStr">
         <is>
@@ -2428,7 +2428,7 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>5000050</v>
+        <v>5000045</v>
       </c>
       <c r="C158" t="inlineStr">
         <is>
@@ -2441,7 +2441,7 @@
         <v>157</v>
       </c>
       <c r="B159" t="n">
-        <v>5000072</v>
+        <v>5000067</v>
       </c>
       <c r="C159" t="inlineStr">
         <is>
@@ -2658,7 +2658,7 @@
         <v>174</v>
       </c>
       <c r="B176" t="n">
-        <v>6000041</v>
+        <v>6000036</v>
       </c>
       <c r="C176" t="inlineStr">
         <is>
@@ -2671,7 +2671,7 @@
         <v>175</v>
       </c>
       <c r="B177" t="n">
-        <v>6000044</v>
+        <v>6000039</v>
       </c>
       <c r="C177" t="inlineStr">
         <is>
@@ -2684,7 +2684,7 @@
         <v>176</v>
       </c>
       <c r="B178" t="n">
-        <v>6000045</v>
+        <v>6000040</v>
       </c>
       <c r="C178" t="inlineStr">
         <is>
@@ -2697,7 +2697,7 @@
         <v>177</v>
       </c>
       <c r="B179" t="n">
-        <v>6000046</v>
+        <v>6000041</v>
       </c>
       <c r="C179" t="inlineStr">
         <is>
@@ -2710,7 +2710,7 @@
         <v>178</v>
       </c>
       <c r="B180" t="n">
-        <v>6000047</v>
+        <v>6000042</v>
       </c>
       <c r="C180" t="inlineStr">
         <is>
@@ -2723,7 +2723,7 @@
         <v>179</v>
       </c>
       <c r="B181" t="n">
-        <v>6000048</v>
+        <v>6000043</v>
       </c>
       <c r="C181" t="inlineStr">
         <is>
@@ -2736,7 +2736,7 @@
         <v>180</v>
       </c>
       <c r="B182" t="n">
-        <v>6000049</v>
+        <v>6000044</v>
       </c>
       <c r="C182" t="inlineStr">
         <is>
@@ -2749,7 +2749,7 @@
         <v>181</v>
       </c>
       <c r="B183" t="n">
-        <v>6000051</v>
+        <v>6000046</v>
       </c>
       <c r="C183" t="inlineStr">
         <is>
@@ -2762,11 +2762,11 @@
         <v>182</v>
       </c>
       <c r="B184" t="n">
-        <v>6000052</v>
+        <v>6000047</v>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>Art 7, Comma 1</t>
+          <t>Art. 20</t>
         </is>
       </c>
     </row>
@@ -2775,11 +2775,11 @@
         <v>183</v>
       </c>
       <c r="B185" t="n">
-        <v>6000053</v>
+        <v>6000048</v>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>Art. 20</t>
+          <t>Art 7, Comma 1</t>
         </is>
       </c>
     </row>
@@ -2788,7 +2788,7 @@
         <v>184</v>
       </c>
       <c r="B186" t="n">
-        <v>6000054</v>
+        <v>6000049</v>
       </c>
       <c r="C186" t="inlineStr">
         <is>
@@ -2801,7 +2801,7 @@
         <v>185</v>
       </c>
       <c r="B187" t="n">
-        <v>6000055</v>
+        <v>6000050</v>
       </c>
       <c r="C187" t="inlineStr">
         <is>
@@ -2814,7 +2814,7 @@
         <v>186</v>
       </c>
       <c r="B188" t="n">
-        <v>6000056</v>
+        <v>6000051</v>
       </c>
       <c r="C188" t="inlineStr">
         <is>
@@ -2827,7 +2827,7 @@
         <v>187</v>
       </c>
       <c r="B189" t="n">
-        <v>6000057</v>
+        <v>6000052</v>
       </c>
       <c r="C189" t="inlineStr">
         <is>
@@ -2840,7 +2840,7 @@
         <v>188</v>
       </c>
       <c r="B190" t="n">
-        <v>6000058</v>
+        <v>6000053</v>
       </c>
       <c r="C190" t="inlineStr">
         <is>
@@ -2853,7 +2853,7 @@
         <v>189</v>
       </c>
       <c r="B191" t="n">
-        <v>6000059</v>
+        <v>6000054</v>
       </c>
       <c r="C191" t="inlineStr">
         <is>
@@ -2866,7 +2866,7 @@
         <v>190</v>
       </c>
       <c r="B192" t="n">
-        <v>6000064</v>
+        <v>6000059</v>
       </c>
       <c r="C192" t="inlineStr">
         <is>
@@ -2879,7 +2879,7 @@
         <v>191</v>
       </c>
       <c r="B193" t="n">
-        <v>6000065</v>
+        <v>6000060</v>
       </c>
       <c r="C193" t="inlineStr">
         <is>
@@ -2892,7 +2892,7 @@
         <v>192</v>
       </c>
       <c r="B194" t="n">
-        <v>6000066</v>
+        <v>6000062</v>
       </c>
       <c r="C194" t="inlineStr">
         <is>
@@ -2905,7 +2905,7 @@
         <v>193</v>
       </c>
       <c r="B195" t="n">
-        <v>6000069</v>
+        <v>6000065</v>
       </c>
       <c r="C195" t="inlineStr">
         <is>
@@ -2918,7 +2918,7 @@
         <v>194</v>
       </c>
       <c r="B196" t="n">
-        <v>6000071</v>
+        <v>6000066</v>
       </c>
       <c r="C196" t="inlineStr">
         <is>
@@ -2931,7 +2931,7 @@
         <v>195</v>
       </c>
       <c r="B197" t="n">
-        <v>6000073</v>
+        <v>6000068</v>
       </c>
       <c r="C197" t="inlineStr">
         <is>
@@ -2944,7 +2944,7 @@
         <v>196</v>
       </c>
       <c r="B198" t="n">
-        <v>6000075</v>
+        <v>6000070</v>
       </c>
       <c r="C198" t="inlineStr">
         <is>
@@ -3070,7 +3070,7 @@
         <v>206</v>
       </c>
       <c r="B208" t="n">
-        <v>7000048</v>
+        <v>7000043</v>
       </c>
       <c r="C208" t="inlineStr">
         <is>
@@ -3083,7 +3083,7 @@
         <v>207</v>
       </c>
       <c r="B209" t="n">
-        <v>7000049</v>
+        <v>7000044</v>
       </c>
       <c r="C209" t="inlineStr">
         <is>
@@ -3300,11 +3300,11 @@
         <v>224</v>
       </c>
       <c r="B226" t="n">
-        <v>8000034</v>
+        <v>8000035</v>
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>SOREU dei Laghi</t>
+          <t>Elemento d'intervento e di supporto dello Stato maggiore federale Protezione della popolazione</t>
         </is>
       </c>
     </row>
@@ -3313,11 +3313,11 @@
         <v>225</v>
       </c>
       <c r="B227" t="n">
-        <v>8000037</v>
+        <v>8000036</v>
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>Le SOREU</t>
+          <t>Legge sulla protezione civile del 26 febbraio 2007</t>
         </is>
       </c>
     </row>
@@ -3330,7 +3330,7 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>Chi siamo</t>
+          <t>Il comando della protezione civile</t>
         </is>
       </c>
     </row>
@@ -3339,11 +3339,11 @@
         <v>227</v>
       </c>
       <c r="B229" t="n">
-        <v>8000040</v>
+        <v>8000039</v>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>Elemento d'intervento e di supporto dello Stato maggiore federale Protezione della popolazione</t>
+          <t>Costruzioni di protezione</t>
         </is>
       </c>
     </row>
@@ -3356,7 +3356,7 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>Legge sulla protezione civile del 26 febbraio 2007</t>
+          <t>Modelli e carte di suscettibilità da frana</t>
         </is>
       </c>
     </row>
@@ -3365,11 +3365,11 @@
         <v>229</v>
       </c>
       <c r="B231" t="n">
-        <v>8000043</v>
+        <v>8000042</v>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>Il comando della protezione civile</t>
+          <t>Legge federale sulla protezione della popolazione e sulla protezione civile del 4 ottobre 2002</t>
         </is>
       </c>
     </row>
@@ -3378,11 +3378,11 @@
         <v>230</v>
       </c>
       <c r="B232" t="n">
-        <v>8000044</v>
+        <v>8000047</v>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>Costruzioni di protezione</t>
+          <t>Legge sulla protezione della popolazione (del 26 febbraio 2007)</t>
         </is>
       </c>
     </row>
@@ -3391,11 +3391,11 @@
         <v>231</v>
       </c>
       <c r="B233" t="n">
-        <v>8000046</v>
+        <v>8000052</v>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>Modelli e carte di suscettibilità da frana</t>
+          <t>Il comando della protezione civile - Personale</t>
         </is>
       </c>
     </row>
@@ -3404,11 +3404,11 @@
         <v>232</v>
       </c>
       <c r="B234" t="n">
-        <v>8000047</v>
+        <v>8000054</v>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>Legge federale sulla protezione della popolazione e sulla protezione civile del 4 ottobre 2002</t>
+          <t>Regolamento sulla protezione della popolazione (RProtPop) (del 18 ottobre 2017)</t>
         </is>
       </c>
     </row>
@@ -3417,11 +3417,11 @@
         <v>233</v>
       </c>
       <c r="B235" t="n">
-        <v>8000053</v>
+        <v>8000058</v>
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>Legge sulla protezione della popolazione (del 26 febbraio 2007)</t>
+          <t>Segnali di allarme in Svizzera</t>
         </is>
       </c>
     </row>
@@ -3430,11 +3430,11 @@
         <v>234</v>
       </c>
       <c r="B236" t="n">
-        <v>8000057</v>
+        <v>8000062</v>
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>Il comando della protezione civile - Personale</t>
+          <t>Servizio della protezione della popolazione</t>
         </is>
       </c>
     </row>
@@ -3443,11 +3443,11 @@
         <v>235</v>
       </c>
       <c r="B237" t="n">
-        <v>8000059</v>
+        <v>8000063</v>
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>Regolamento sulla protezione della popolazione (RProtPop) (del 18 ottobre 2017)</t>
+          <t>Dipartimento</t>
         </is>
       </c>
     </row>
@@ -3456,11 +3456,11 @@
         <v>236</v>
       </c>
       <c r="B238" t="n">
-        <v>8000063</v>
+        <v>8000065</v>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>Segnali di allarme in Svizzera</t>
+          <t>-- documento confronto normativa -- wp 3.2 gestisco -- da completare</t>
         </is>
       </c>
     </row>
@@ -3469,11 +3469,11 @@
         <v>237</v>
       </c>
       <c r="B239" t="n">
-        <v>8000066</v>
+        <v>8000070</v>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>Servizio della protezione della popolazione</t>
+          <t>-- -- documento confronto normativa -- wp 3.2 gestisco -- da completare</t>
         </is>
       </c>
     </row>
@@ -3482,11 +3482,11 @@
         <v>238</v>
       </c>
       <c r="B240" t="n">
-        <v>8000068</v>
+        <v>8000073</v>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>Dipartimento</t>
+          <t>Le SOREU</t>
         </is>
       </c>
     </row>
@@ -3495,11 +3495,11 @@
         <v>239</v>
       </c>
       <c r="B241" t="n">
-        <v>8000069</v>
+        <v>8000074</v>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>-- documento confronto normativa -- wp 3.2 gestisco -- da completare</t>
+          <t>SOREU dei Laghi</t>
         </is>
       </c>
     </row>
@@ -3512,7 +3512,7 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>-- -- documento confronto normativa -- wp 3.2 gestisco -- da completare</t>
+          <t>Chi siamo</t>
         </is>
       </c>
     </row>
@@ -3621,11 +3621,11 @@
         <v>249</v>
       </c>
       <c r="B251" t="n">
-        <v>9000035</v>
+        <v>9000041</v>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>Alberto Bruno, Funzionario della protezione civile di regione lombardia</t>
+          <t>IRPI</t>
         </is>
       </c>
     </row>
@@ -3634,11 +3634,11 @@
         <v>250</v>
       </c>
       <c r="B252" t="n">
-        <v>9000046</v>
+        <v>9000045</v>
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>IRPI</t>
+          <t>Confederazion elvetica</t>
         </is>
       </c>
     </row>
@@ -3647,11 +3647,11 @@
         <v>251</v>
       </c>
       <c r="B253" t="n">
-        <v>9000050</v>
+        <v>9000052</v>
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>Confederazion elvetica</t>
+          <t>Ufficio Federale della Protezione della Popolazione</t>
         </is>
       </c>
     </row>
@@ -3660,11 +3660,11 @@
         <v>252</v>
       </c>
       <c r="B254" t="n">
-        <v>9000057</v>
+        <v>9000062</v>
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>Ufficio Federale della Protezione della Popolazione</t>
+          <t>Repubblica e Cantone Ticino</t>
         </is>
       </c>
     </row>
@@ -3673,11 +3673,11 @@
         <v>253</v>
       </c>
       <c r="B255" t="n">
-        <v>9000066</v>
+        <v>9000065</v>
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>Repubblica e Cantone Ticino</t>
+          <t>Tommaso Sansone</t>
         </is>
       </c>
     </row>
@@ -3686,11 +3686,11 @@
         <v>254</v>
       </c>
       <c r="B256" t="n">
-        <v>9000069</v>
+        <v>9000067</v>
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>Tommaso Sansone</t>
+          <t>Tommaso sansone</t>
         </is>
       </c>
     </row>
@@ -3703,7 +3703,7 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>Tommaso sansone</t>
+          <t>Alberto Bruno, Funzionario della protezione civile di regione lombardia</t>
         </is>
       </c>
     </row>
@@ -3877,11 +3877,11 @@
         <v>269</v>
       </c>
       <c r="B271" t="n">
-        <v>10000034</v>
+        <v>10000036</v>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>Areu Lombardia</t>
+          <t>Repubblica e Cantone Ticino</t>
         </is>
       </c>
     </row>
@@ -3890,11 +3890,11 @@
         <v>270</v>
       </c>
       <c r="B272" t="n">
-        <v>10000038</v>
+        <v>10000041</v>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>Repubblica e Canton Ticino</t>
+          <t>IRPI CNR</t>
         </is>
       </c>
     </row>
@@ -3903,11 +3903,11 @@
         <v>271</v>
       </c>
       <c r="B273" t="n">
-        <v>10000041</v>
+        <v>10000045</v>
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>Repubblica e Cantone Ticino</t>
+          <t>Confederazione elvetica</t>
         </is>
       </c>
     </row>
@@ -3916,11 +3916,11 @@
         <v>272</v>
       </c>
       <c r="B274" t="n">
-        <v>10000046</v>
+        <v>10000073</v>
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>IRPI CNR</t>
+          <t>Areu Lombardia</t>
         </is>
       </c>
     </row>
@@ -3929,11 +3929,11 @@
         <v>273</v>
       </c>
       <c r="B275" t="n">
-        <v>10000050</v>
+        <v>10000075</v>
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>Confederazione elvetica</t>
+          <t>Repubblica e Canton Ticino</t>
         </is>
       </c>
     </row>
@@ -4111,7 +4111,7 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>https://www.areu.lombardia.it/web/home/soreu-dei-laghi</t>
+          <t>https://www.naz.ch/index_it.html</t>
         </is>
       </c>
     </row>
@@ -4124,7 +4124,7 @@
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>http://www.protezionecivile.gov.it/servizio-nazionale/strutture-operative/volontariato</t>
+          <t>https://www.naz.ch/it/naz/eo.html</t>
         </is>
       </c>
     </row>
@@ -4133,11 +4133,11 @@
         <v>289</v>
       </c>
       <c r="B291" t="n">
-        <v>11000037</v>
+        <v>11000036</v>
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>https://www.areu.lombardia.it/web/home/soreu</t>
+          <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/raccolta-leggi/legge/num/44</t>
         </is>
       </c>
     </row>
@@ -4150,7 +4150,7 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>https://www4.ti.ch/di/smpp/chi-siamo/presentazione/</t>
+          <t>https://www.babs.admin.ch/it/zs/org/kdo.html</t>
         </is>
       </c>
     </row>
@@ -4163,7 +4163,7 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>https://www.naz.ch/index_it.html</t>
+          <t>https://www.babs.admin.ch/it/aufgabenbabs/schutzbauten.html</t>
         </is>
       </c>
     </row>
@@ -4176,7 +4176,7 @@
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>https://www.naz.ch/it/naz/eo.html</t>
+          <t>http://www.protezionecivile.gov.it/dipartimento</t>
         </is>
       </c>
     </row>
@@ -4189,7 +4189,7 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/raccolta-leggi/legge/num/44</t>
+          <t>http://www.irpi.cnr.it/focus/suscettibilita-da-frana/</t>
         </is>
       </c>
     </row>
@@ -4198,11 +4198,11 @@
         <v>294</v>
       </c>
       <c r="B296" t="n">
-        <v>11000043</v>
+        <v>11000042</v>
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>https://www.babs.admin.ch/it/zs/org/kdo.html</t>
+          <t>https://www.admin.ch/opc/it/classified-compilation/20011872/201701010000/520.1.pdf</t>
         </is>
       </c>
     </row>
@@ -4211,11 +4211,11 @@
         <v>295</v>
       </c>
       <c r="B297" t="n">
-        <v>11000044</v>
+        <v>11000043</v>
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>https://www.babs.admin.ch/it/aufgabenbabs/schutzbauten.html</t>
+          <t>https://www.gazzettaufficiale.it/eli/id/2018/1/22/18G00011/sg</t>
         </is>
       </c>
     </row>
@@ -4224,11 +4224,11 @@
         <v>296</v>
       </c>
       <c r="B298" t="n">
-        <v>11000045</v>
+        <v>11000047</v>
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>http://www.protezionecivile.gov.it/dipartimento</t>
+          <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/raccolta-leggi/legge/num/48</t>
         </is>
       </c>
     </row>
@@ -4237,11 +4237,11 @@
         <v>297</v>
       </c>
       <c r="B299" t="n">
-        <v>11000046</v>
+        <v>11000052</v>
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>http://www.irpi.cnr.it/focus/suscettibilita-da-frana/</t>
+          <t>https://www.babs.admin.ch/content/babs-internet/it/publikservice/downloads/unterlagen-ausbildung/_jcr_content/contentPar/accordion_1920886228/accordionItems/kommando_zivilschutz/accordionPar/downloadlist_copy/downloadItems/829_1459931125997.download/personal170191103it.pdf</t>
         </is>
       </c>
     </row>
@@ -4250,11 +4250,11 @@
         <v>298</v>
       </c>
       <c r="B300" t="n">
-        <v>11000047</v>
+        <v>11000054</v>
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>https://www.admin.ch/opc/it/classified-compilation/20011872/201701010000/520.1.pdf</t>
+          <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/index/nuovafinestra/atto/49/volume/5%20SICUREZZA/numLegge/500.110</t>
         </is>
       </c>
     </row>
@@ -4263,11 +4263,11 @@
         <v>299</v>
       </c>
       <c r="B301" t="n">
-        <v>11000048</v>
+        <v>11000057</v>
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>https://www.gazzettaufficiale.it/eli/id/2018/1/22/18G00011/sg</t>
+          <t>http://www.protezionecivile.gov.it/servizio-nazionale/strutture-operative/volontariato</t>
         </is>
       </c>
     </row>
@@ -4276,11 +4276,11 @@
         <v>300</v>
       </c>
       <c r="B302" t="n">
-        <v>11000053</v>
+        <v>11000058</v>
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/raccolta-leggi/legge/num/48</t>
+          <t>https://www.ch.ch/it/allarme-sirene/</t>
         </is>
       </c>
     </row>
@@ -4289,11 +4289,11 @@
         <v>301</v>
       </c>
       <c r="B303" t="n">
-        <v>11000057</v>
+        <v>11000062</v>
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>https://www.babs.admin.ch/content/babs-internet/it/publikservice/downloads/unterlagen-ausbildung/_jcr_content/contentPar/accordion_1920886228/accordionItems/kommando_zivilschutz/accordionPar/downloadlist_copy/downloadItems/829_1459931125997.download/personal170191103it.pdf</t>
+          <t>https://www4.ti.ch/di/smpp/chi-siamo/servizio-della-protezione-della-popolazione/</t>
         </is>
       </c>
     </row>
@@ -4302,11 +4302,11 @@
         <v>302</v>
       </c>
       <c r="B304" t="n">
-        <v>11000059</v>
+        <v>11000068</v>
       </c>
       <c r="C304" t="inlineStr">
         <is>
-          <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/index/nuovafinestra/atto/49/volume/5%20SICUREZZA/numLegge/500.110</t>
+          <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/raccolta-leggi/pdfatto/atto/48</t>
         </is>
       </c>
     </row>
@@ -4315,11 +4315,11 @@
         <v>303</v>
       </c>
       <c r="B305" t="n">
-        <v>11000063</v>
+        <v>11000073</v>
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>https://www.ch.ch/it/allarme-sirene/</t>
+          <t>https://www.areu.lombardia.it/web/home/soreu</t>
         </is>
       </c>
     </row>
@@ -4328,11 +4328,11 @@
         <v>304</v>
       </c>
       <c r="B306" t="n">
-        <v>11000066</v>
+        <v>11000074</v>
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>https://www4.ti.ch/di/smpp/chi-siamo/servizio-della-protezione-della-popolazione/</t>
+          <t>https://www.areu.lombardia.it/web/home/soreu-dei-laghi</t>
         </is>
       </c>
     </row>
@@ -4341,11 +4341,11 @@
         <v>305</v>
       </c>
       <c r="B307" t="n">
-        <v>11000073</v>
+        <v>11000075</v>
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>https://m3.ti.ch/CAN/RLeggi/public/index.php/raccolta-leggi/pdfatto/atto/48</t>
+          <t>https://www4.ti.ch/di/smpp/chi-siamo/presentazione/</t>
         </is>
       </c>
     </row>
@@ -4376,7 +4376,7 @@
         <v>308</v>
       </c>
       <c r="B310" t="n">
-        <v>12000041</v>
+        <v>12000036</v>
       </c>
       <c r="C310" t="inlineStr">
         <is>
@@ -4389,7 +4389,7 @@
         <v>309</v>
       </c>
       <c r="B311" t="n">
-        <v>12000047</v>
+        <v>12000042</v>
       </c>
       <c r="C311" t="inlineStr">
         <is>
@@ -4402,7 +4402,7 @@
         <v>310</v>
       </c>
       <c r="B312" t="n">
-        <v>12000049</v>
+        <v>12000044</v>
       </c>
       <c r="C312" t="inlineStr">
         <is>
@@ -4415,7 +4415,7 @@
         <v>311</v>
       </c>
       <c r="B313" t="n">
-        <v>12000052</v>
+        <v>12000047</v>
       </c>
       <c r="C313" t="inlineStr">
         <is>
@@ -4428,7 +4428,7 @@
         <v>312</v>
       </c>
       <c r="B314" t="n">
-        <v>12000066</v>
+        <v>12000061</v>
       </c>
       <c r="C314" t="inlineStr">
         <is>
@@ -4442,7 +4442,7 @@
         <v>313</v>
       </c>
       <c r="B315" t="n">
-        <v>12000069</v>
+        <v>12000064</v>
       </c>
       <c r="C315" t="inlineStr">
         <is>
@@ -4455,7 +4455,7 @@
         <v>314</v>
       </c>
       <c r="B316" t="n">
-        <v>12000075</v>
+        <v>12000070</v>
       </c>
       <c r="C316" t="inlineStr">
         <is>
@@ -4537,7 +4537,7 @@
         <v>13000034</v>
       </c>
       <c r="C323" s="2" t="n">
-        <v>43844</v>
+        <v>43656</v>
       </c>
     </row>
     <row r="324">
@@ -4545,10 +4545,10 @@
         <v>322</v>
       </c>
       <c r="B324" t="n">
-        <v>13000035</v>
+        <v>13000039</v>
       </c>
       <c r="C324" s="2" t="n">
-        <v>43804</v>
+        <v>43657</v>
       </c>
     </row>
     <row r="325">
@@ -4556,10 +4556,10 @@
         <v>323</v>
       </c>
       <c r="B325" t="n">
-        <v>13000036</v>
+        <v>13000040</v>
       </c>
       <c r="C325" s="2" t="n">
-        <v>43774</v>
+        <v>43767</v>
       </c>
     </row>
     <row r="326">
@@ -4567,10 +4567,10 @@
         <v>324</v>
       </c>
       <c r="B326" t="n">
-        <v>13000038</v>
+        <v>13000041</v>
       </c>
       <c r="C326" s="2" t="n">
-        <v>43845</v>
+        <v>43731</v>
       </c>
     </row>
     <row r="327">
@@ -4578,10 +4578,10 @@
         <v>325</v>
       </c>
       <c r="B327" t="n">
-        <v>13000039</v>
+        <v>13000042</v>
       </c>
       <c r="C327" s="2" t="n">
-        <v>43656</v>
+        <v>43766</v>
       </c>
     </row>
     <row r="328">
@@ -4589,10 +4589,10 @@
         <v>326</v>
       </c>
       <c r="B328" t="n">
-        <v>13000040</v>
+        <v>13000061</v>
       </c>
       <c r="C328" s="2" t="n">
-        <v>43767</v>
+        <v>43815</v>
       </c>
     </row>
     <row r="329">
@@ -4600,10 +4600,10 @@
         <v>327</v>
       </c>
       <c r="B329" t="n">
-        <v>13000044</v>
+        <v>13000063</v>
       </c>
       <c r="C329" s="2" t="n">
-        <v>43657</v>
+        <v>43817</v>
       </c>
     </row>
     <row r="330">
@@ -4611,10 +4611,10 @@
         <v>328</v>
       </c>
       <c r="B330" t="n">
-        <v>13000046</v>
+        <v>13000064</v>
       </c>
       <c r="C330" s="2" t="n">
-        <v>43731</v>
+        <v>43780</v>
       </c>
     </row>
     <row r="331">
@@ -4622,10 +4622,10 @@
         <v>329</v>
       </c>
       <c r="B331" t="n">
-        <v>13000047</v>
+        <v>13000071</v>
       </c>
       <c r="C331" s="2" t="n">
-        <v>43766</v>
+        <v>43774</v>
       </c>
     </row>
     <row r="332">
@@ -4633,10 +4633,10 @@
         <v>330</v>
       </c>
       <c r="B332" t="n">
-        <v>13000066</v>
+        <v>13000072</v>
       </c>
       <c r="C332" s="2" t="n">
-        <v>43815</v>
+        <v>43804</v>
       </c>
     </row>
     <row r="333">
@@ -4644,10 +4644,10 @@
         <v>331</v>
       </c>
       <c r="B333" t="n">
-        <v>13000068</v>
+        <v>13000073</v>
       </c>
       <c r="C333" s="2" t="n">
-        <v>43817</v>
+        <v>43844</v>
       </c>
     </row>
     <row r="334">
@@ -4655,10 +4655,10 @@
         <v>332</v>
       </c>
       <c r="B334" t="n">
-        <v>13000069</v>
+        <v>13000075</v>
       </c>
       <c r="C334" s="2" t="n">
-        <v>43780</v>
+        <v>43845</v>
       </c>
     </row>
     <row r="335">
@@ -5086,7 +5086,7 @@
       </c>
       <c r="C367" t="inlineStr">
         <is>
-          <t>ITCH00000</t>
+          <t>ITCH00001</t>
         </is>
       </c>
     </row>
@@ -5095,11 +5095,11 @@
         <v>366</v>
       </c>
       <c r="B368" t="n">
-        <v>14000039</v>
+        <v>14000035</v>
       </c>
       <c r="C368" t="inlineStr">
         <is>
-          <t>ITCH00001</t>
+          <t>ITCH00002</t>
         </is>
       </c>
     </row>
@@ -5108,11 +5108,11 @@
         <v>367</v>
       </c>
       <c r="B369" t="n">
-        <v>14000040</v>
+        <v>14000036</v>
       </c>
       <c r="C369" t="inlineStr">
         <is>
-          <t>ITCH00002</t>
+          <t>ITCH00003</t>
         </is>
       </c>
     </row>
@@ -5121,11 +5121,11 @@
         <v>368</v>
       </c>
       <c r="B370" t="n">
-        <v>14000041</v>
+        <v>14000038</v>
       </c>
       <c r="C370" t="inlineStr">
         <is>
-          <t>ITCH00003</t>
+          <t>ITCH00004</t>
         </is>
       </c>
     </row>
@@ -5134,11 +5134,11 @@
         <v>369</v>
       </c>
       <c r="B371" t="n">
-        <v>14000043</v>
+        <v>14000039</v>
       </c>
       <c r="C371" t="inlineStr">
         <is>
-          <t>ITCH00004</t>
+          <t>ITCH00005</t>
         </is>
       </c>
     </row>
@@ -5147,11 +5147,11 @@
         <v>370</v>
       </c>
       <c r="B372" t="n">
-        <v>14000044</v>
+        <v>14000040</v>
       </c>
       <c r="C372" t="inlineStr">
         <is>
-          <t>ITCH00005</t>
+          <t>ITCH00006</t>
         </is>
       </c>
     </row>
@@ -5160,11 +5160,11 @@
         <v>371</v>
       </c>
       <c r="B373" t="n">
-        <v>14000045</v>
+        <v>14000041</v>
       </c>
       <c r="C373" t="inlineStr">
         <is>
-          <t>ITCH00006</t>
+          <t>ITCH00007</t>
         </is>
       </c>
     </row>
@@ -5173,11 +5173,11 @@
         <v>372</v>
       </c>
       <c r="B374" t="n">
-        <v>14000046</v>
+        <v>14000042</v>
       </c>
       <c r="C374" t="inlineStr">
         <is>
-          <t>ITCH00007</t>
+          <t>ITCH00009</t>
         </is>
       </c>
     </row>
@@ -5186,11 +5186,11 @@
         <v>373</v>
       </c>
       <c r="B375" t="n">
-        <v>14000047</v>
+        <v>14000044</v>
       </c>
       <c r="C375" t="inlineStr">
         <is>
-          <t>ITCH00009</t>
+          <t>ITCH00010</t>
         </is>
       </c>
     </row>
@@ -5199,11 +5199,11 @@
         <v>374</v>
       </c>
       <c r="B376" t="n">
-        <v>14000049</v>
+        <v>14000046</v>
       </c>
       <c r="C376" t="inlineStr">
         <is>
-          <t>ITCH00010</t>
+          <t>ITCH00011</t>
         </is>
       </c>
     </row>
@@ -5212,11 +5212,11 @@
         <v>375</v>
       </c>
       <c r="B377" t="n">
-        <v>14000051</v>
+        <v>14000047</v>
       </c>
       <c r="C377" t="inlineStr">
         <is>
-          <t>ITCH00011</t>
+          <t>ITCH00012</t>
         </is>
       </c>
     </row>
@@ -5225,11 +5225,11 @@
         <v>376</v>
       </c>
       <c r="B378" t="n">
-        <v>14000052</v>
+        <v>14000049</v>
       </c>
       <c r="C378" t="inlineStr">
         <is>
-          <t>ITCH00012</t>
+          <t>ITCH00013</t>
         </is>
       </c>
     </row>
@@ -5238,11 +5238,11 @@
         <v>377</v>
       </c>
       <c r="B379" t="n">
-        <v>14000054</v>
+        <v>14000050</v>
       </c>
       <c r="C379" t="inlineStr">
         <is>
-          <t>ITCH00013</t>
+          <t>ITCH00014</t>
         </is>
       </c>
     </row>
@@ -5251,11 +5251,11 @@
         <v>378</v>
       </c>
       <c r="B380" t="n">
-        <v>14000055</v>
+        <v>14000051</v>
       </c>
       <c r="C380" t="inlineStr">
         <is>
-          <t>ITCH00014</t>
+          <t>ITCH00015</t>
         </is>
       </c>
     </row>
@@ -5264,11 +5264,11 @@
         <v>379</v>
       </c>
       <c r="B381" t="n">
-        <v>14000056</v>
+        <v>14000052</v>
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>ITCH00015</t>
+          <t>ITCH00016</t>
         </is>
       </c>
     </row>
@@ -5277,11 +5277,11 @@
         <v>380</v>
       </c>
       <c r="B382" t="n">
-        <v>14000057</v>
+        <v>14000053</v>
       </c>
       <c r="C382" t="inlineStr">
         <is>
-          <t>ITCH00016</t>
+          <t>ITCH00017</t>
         </is>
       </c>
     </row>
@@ -5290,11 +5290,11 @@
         <v>381</v>
       </c>
       <c r="B383" t="n">
-        <v>14000058</v>
+        <v>14000054</v>
       </c>
       <c r="C383" t="inlineStr">
         <is>
-          <t>ITCH00017</t>
+          <t>ITCH00018</t>
         </is>
       </c>
     </row>
@@ -5303,11 +5303,11 @@
         <v>382</v>
       </c>
       <c r="B384" t="n">
-        <v>14000059</v>
+        <v>14000055</v>
       </c>
       <c r="C384" t="inlineStr">
         <is>
-          <t>ITCH00018</t>
+          <t>ITCH00019</t>
         </is>
       </c>
     </row>
@@ -5316,11 +5316,11 @@
         <v>383</v>
       </c>
       <c r="B385" t="n">
-        <v>14000060</v>
+        <v>14000056</v>
       </c>
       <c r="C385" t="inlineStr">
         <is>
-          <t>ITCH00019</t>
+          <t>ITCH00020</t>
         </is>
       </c>
     </row>
@@ -5329,11 +5329,11 @@
         <v>384</v>
       </c>
       <c r="B386" t="n">
-        <v>14000061</v>
+        <v>14000057</v>
       </c>
       <c r="C386" t="inlineStr">
         <is>
-          <t>ITCH00020</t>
+          <t>ITCH00021</t>
         </is>
       </c>
     </row>
@@ -5342,11 +5342,11 @@
         <v>385</v>
       </c>
       <c r="B387" t="n">
-        <v>14000062</v>
+        <v>14000058</v>
       </c>
       <c r="C387" t="inlineStr">
         <is>
-          <t>ITCH00021</t>
+          <t>ITCH00022</t>
         </is>
       </c>
     </row>
@@ -5355,11 +5355,11 @@
         <v>386</v>
       </c>
       <c r="B388" t="n">
-        <v>14000063</v>
+        <v>14000059</v>
       </c>
       <c r="C388" t="inlineStr">
         <is>
-          <t>ITCH00022</t>
+          <t>ITCH00023</t>
         </is>
       </c>
     </row>
@@ -5368,11 +5368,11 @@
         <v>387</v>
       </c>
       <c r="B389" t="n">
-        <v>14000064</v>
+        <v>14000060</v>
       </c>
       <c r="C389" t="inlineStr">
         <is>
-          <t>ITCH00023</t>
+          <t>ITCH00024</t>
         </is>
       </c>
     </row>
@@ -5381,11 +5381,11 @@
         <v>388</v>
       </c>
       <c r="B390" t="n">
-        <v>14000065</v>
+        <v>14000061</v>
       </c>
       <c r="C390" t="inlineStr">
         <is>
-          <t>ITCH00024</t>
+          <t>ITCH00025</t>
         </is>
       </c>
     </row>
@@ -5394,11 +5394,11 @@
         <v>389</v>
       </c>
       <c r="B391" t="n">
-        <v>14000066</v>
+        <v>14000063</v>
       </c>
       <c r="C391" t="inlineStr">
         <is>
-          <t>ITCH00025</t>
+          <t>ITCH00026</t>
         </is>
       </c>
     </row>
@@ -5407,11 +5407,11 @@
         <v>390</v>
       </c>
       <c r="B392" t="n">
-        <v>14000068</v>
+        <v>14000064</v>
       </c>
       <c r="C392" t="inlineStr">
         <is>
-          <t>ITCH00026</t>
+          <t>ITCH00027</t>
         </is>
       </c>
     </row>
@@ -5420,11 +5420,11 @@
         <v>391</v>
       </c>
       <c r="B393" t="n">
-        <v>14000069</v>
+        <v>14000066</v>
       </c>
       <c r="C393" t="inlineStr">
         <is>
-          <t>ITCH00027</t>
+          <t>ITCH00028</t>
         </is>
       </c>
     </row>
@@ -5433,11 +5433,11 @@
         <v>392</v>
       </c>
       <c r="B394" t="n">
-        <v>14000071</v>
+        <v>14000068</v>
       </c>
       <c r="C394" t="inlineStr">
         <is>
-          <t>ITCH00028</t>
+          <t>ITCH00029</t>
         </is>
       </c>
     </row>
@@ -5446,11 +5446,11 @@
         <v>393</v>
       </c>
       <c r="B395" t="n">
-        <v>14000073</v>
+        <v>14000069</v>
       </c>
       <c r="C395" t="inlineStr">
         <is>
-          <t>ITCH00029</t>
+          <t>ITCH00030</t>
         </is>
       </c>
     </row>
@@ -5459,11 +5459,11 @@
         <v>394</v>
       </c>
       <c r="B396" t="n">
-        <v>14000074</v>
+        <v>14000070</v>
       </c>
       <c r="C396" t="inlineStr">
         <is>
-          <t>ITCH00030</t>
+          <t>ITCH00031</t>
         </is>
       </c>
     </row>
@@ -5472,11 +5472,11 @@
         <v>395</v>
       </c>
       <c r="B397" t="n">
-        <v>14000075</v>
+        <v>14000071</v>
       </c>
       <c r="C397" t="inlineStr">
         <is>
-          <t>ITCH00031</t>
+          <t>ITCH00032</t>
         </is>
       </c>
     </row>
@@ -5485,11 +5485,11 @@
         <v>396</v>
       </c>
       <c r="B398" t="n">
-        <v>14000076</v>
+        <v>14000072</v>
       </c>
       <c r="C398" t="inlineStr">
         <is>
-          <t>ITCH00040</t>
+          <t>ITCH00033</t>
         </is>
       </c>
     </row>
@@ -5498,9 +5498,61 @@
         <v>397</v>
       </c>
       <c r="B399" t="n">
+        <v>14000073</v>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>ITCH00034</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" s="1" t="n">
+        <v>398</v>
+      </c>
+      <c r="B400" t="n">
+        <v>14000074</v>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>ITCH00035</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" s="1" t="n">
+        <v>399</v>
+      </c>
+      <c r="B401" t="n">
+        <v>14000075</v>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>ITCH00036</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" s="1" t="n">
+        <v>400</v>
+      </c>
+      <c r="B402" t="n">
+        <v>14000076</v>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>ITCH00040</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" s="1" t="n">
+        <v>401</v>
+      </c>
+      <c r="B403" t="n">
         <v>15000001</v>
       </c>
-      <c r="C399" t="inlineStr">
+      <c r="C403" t="inlineStr">
         <is>
           <t>show</t>
         </is>

</xml_diff>